<commit_message>
adding retirement list code and files
</commit_message>
<xml_diff>
--- a/PewlettHackard_DBD_Schema.xlsx
+++ b/PewlettHackard_DBD_Schema.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliaheuer/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliaheuer/Desktop/DataAnalyticsCourseWork/Analysis_Projects_Folder/Pewlett-Hackard-Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C70F064-ACAC-2840-AFB0-9C14E0B55E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5720BFFA-99E8-AC4B-A94A-30794BD52709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{0F5CD544-E38D-924E-B989-73BD8B8E63C2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t xml:space="preserve">Departments </t>
   </si>
@@ -93,9 +93,6 @@
     <t>emp_no varchar pk fk -&lt; Salaries.emp_no</t>
   </si>
   <si>
-    <t>title varchar</t>
-  </si>
-  <si>
     <t>to_date date</t>
   </si>
   <si>
@@ -114,7 +111,16 @@
     <t>dept_no varchar pk fk - Departments.dept_no</t>
   </si>
   <si>
-    <t>emp_no fk - Employees.emp_no</t>
+    <t xml:space="preserve">emp_no fk - Employees.emp_no pk </t>
+  </si>
+  <si>
+    <t xml:space="preserve">from_date date </t>
+  </si>
+  <si>
+    <t>title varchar pk</t>
+  </si>
+  <si>
+    <t>from_date date pk</t>
   </si>
 </sst>
 </file>
@@ -468,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82AA87EA-7E46-E745-93D1-832496C2B86C}">
   <dimension ref="A1:A41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A42"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -584,22 +590,22 @@
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
@@ -609,12 +615,12 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
@@ -624,12 +630,12 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
@@ -639,17 +645,17 @@
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>